<commit_message>
Added some vocabs and misspelled words.
</commit_message>
<xml_diff>
--- a/Vocabs.xlsx
+++ b/Vocabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D31381D-F94C-413C-B886-237F7F086006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E5A2E1-7EB8-40F6-BD17-AC7D5059B243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>NULL</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>very deep/huge</t>
+  </si>
+  <si>
+    <t>coup de grâce</t>
+  </si>
+  <si>
+    <t>a final blow to kill someone wounded as Mercy</t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,8 +925,12 @@
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>

</xml_diff>

<commit_message>
Added Vocabs and misspelled word.
</commit_message>
<xml_diff>
--- a/Vocabs.xlsx
+++ b/Vocabs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206AE323-44B2-45D0-B3AC-F90241E5CDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B7040D-7724-430D-B321-BFD4653FA41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>NULL</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>a (conincedent) circumstance that just happened</t>
+  </si>
+  <si>
+    <t>commence</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>commencement</t>
+  </si>
+  <si>
+    <t>Graduation Ceremony/Day</t>
   </si>
 </sst>
 </file>
@@ -602,7 +614,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,7 +623,7 @@
     <col min="2" max="2" width="14.54296875" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="4.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
     <col min="6" max="6" width="39.6328125" customWidth="1"/>
     <col min="7" max="7" width="4.90625" customWidth="1"/>
     <col min="8" max="8" width="13.7265625" customWidth="1"/>
@@ -854,8 +866,12 @@
         <v>17</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -874,8 +890,12 @@
         <v>19</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>

</xml_diff>

<commit_message>
Practiced Confusing Words and added some vocabs.
</commit_message>
<xml_diff>
--- a/Vocabs.xlsx
+++ b/Vocabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58312301-95FE-40B6-88ED-11A5C1F43117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7FD497-BDB0-47BB-891A-7145A8DD55CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
   <si>
     <t>NULL</t>
   </si>
@@ -286,13 +286,25 @@
   </si>
   <si>
     <t>behave in a calm/cofident way</t>
+  </si>
+  <si>
+    <t>pertain</t>
+  </si>
+  <si>
+    <t>realated to sth</t>
+  </si>
+  <si>
+    <t>procession</t>
+  </si>
+  <si>
+    <t>line of MovingPeople at a ceremony/event</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +333,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,8 +365,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -354,14 +379,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,13 +416,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -695,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE2BE65-1CC2-4D31-AB72-F2E4F74D8764}">
-  <dimension ref="B2:O33"/>
+  <dimension ref="A2:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,38 +767,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -897,8 +943,12 @@
         <v>52</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -921,8 +971,12 @@
         <v>51</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1100,7 +1154,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1124,7 +1178,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1148,7 +1202,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1172,7 +1226,7 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>35</v>
       </c>
@@ -1196,7 +1250,7 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>36</v>
       </c>
@@ -1220,7 +1274,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1244,7 +1298,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3" t="s">
         <v>41</v>
       </c>
@@ -1268,15 +1322,16 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+    <row r="24" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="4"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1284,7 +1339,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
@@ -1300,7 +1355,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
@@ -1316,37 +1371,37 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D27" s="4"/>
       <c r="G27" s="4"/>
       <c r="J27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D28" s="4"/>
       <c r="G28" s="4"/>
       <c r="J28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D29" s="4"/>
       <c r="G29" s="4"/>
       <c r="J29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D30" s="4"/>
       <c r="G30" s="4"/>
       <c r="J30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D31" s="4"/>
       <c r="G31" s="4"/>
       <c r="J31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D32" s="4"/>
       <c r="G32" s="4"/>
       <c r="J32" s="4"/>
@@ -1354,8 +1409,88 @@
     </row>
     <row r="33" spans="4:13" x14ac:dyDescent="0.35">
       <c r="D33" s="4"/>
+      <c r="G33" s="4"/>
       <c r="J33" s="4"/>
       <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.35">
+      <c r="D48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G49" s="4"/>
+      <c r="J49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Practiced IELTS 11 Test 3 and 4
</commit_message>
<xml_diff>
--- a/Vocabs.xlsx
+++ b/Vocabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FC30DA-66E1-4E73-97D2-3F0AE7366AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6061A-BCF4-4258-A3B6-340AB9A8BF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>NULL</t>
   </si>
@@ -303,7 +303,13 @@
     <t>omit</t>
   </si>
   <si>
-    <t>to not include sth</t>
+    <t>intuitive</t>
+  </si>
+  <si>
+    <t>leave out / to not include sth</t>
+  </si>
+  <si>
+    <t>feeling of knowing sth with being able to explain</t>
   </si>
 </sst>
 </file>
@@ -750,7 +756,7 @@
   <dimension ref="A2:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,7 +1015,7 @@
         <v>91</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
@@ -1033,8 +1039,12 @@
         <v>56</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>

</xml_diff>

<commit_message>
Practiced Context and meaning Exercise 1.
</commit_message>
<xml_diff>
--- a/Vocabs.xlsx
+++ b/Vocabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31CB078-3541-48DC-98AA-C1F87322479E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5837C62-DD96-4D74-B228-95C2D0F5D02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="103">
   <si>
     <t>NULL</t>
   </si>
@@ -322,6 +322,18 @@
   </si>
   <si>
     <t>stay somewhere for a long time</t>
+  </si>
+  <si>
+    <t>trivial</t>
+  </si>
+  <si>
+    <t>small | not important/matter</t>
+  </si>
+  <si>
+    <t>patent</t>
+  </si>
+  <si>
+    <t>obvious | legal right to sell sth/invention</t>
   </si>
 </sst>
 </file>
@@ -768,7 +780,7 @@
   <dimension ref="A2:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1137,8 +1149,12 @@
         <v>74</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1161,8 +1177,12 @@
         <v>75</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="J15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>

</xml_diff>

<commit_message>
Added Vocabs from Context and Meaning 2.
</commit_message>
<xml_diff>
--- a/Vocabs.xlsx
+++ b/Vocabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED7A966-2B64-48E0-A696-E9EF0A821356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB1D6C-9B58-4DA2-AFD6-3E53261B24F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="113">
   <si>
     <t>NULL</t>
   </si>
@@ -340,6 +340,30 @@
   </si>
   <si>
     <t>smooth/shiny hair (or) attractive/expensive car</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeopardize </t>
+  </si>
+  <si>
+    <t>risk damaging or destroying sth important</t>
+  </si>
+  <si>
+    <t>hinder</t>
+  </si>
+  <si>
+    <t>stop sth (from developing/progressing)</t>
+  </si>
+  <si>
+    <t>disparate</t>
+  </si>
+  <si>
+    <t>having many differences</t>
+  </si>
+  <si>
+    <t>coarse</t>
+  </si>
+  <si>
+    <t>rough and hard</t>
   </si>
 </sst>
 </file>
@@ -786,7 +810,7 @@
   <dimension ref="A2:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,8 +1263,12 @@
         <v>78</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1263,8 +1291,12 @@
         <v>79</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1287,8 +1319,12 @@
         <v>80</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="J19" s="4"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1311,8 +1347,12 @@
         <v>81</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="J20" s="4"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>

</xml_diff>